<commit_message>
Float32Array_Int32Array to spec (slow)
</commit_message>
<xml_diff>
--- a/packed conversions.xlsx
+++ b/packed conversions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachb\git\tacvt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBEDDC6-D087-44B2-B104-9534B5036FA3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E383B6-8A0E-4DF9-9A1A-9779F5352AAF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12150" yWindow="-21435" windowWidth="25050" windowHeight="15465" xr2:uid="{03DD5425-0ECE-42AD-87FB-24C50220D827}"/>
+    <workbookView xWindow="2674" yWindow="857" windowWidth="25055" windowHeight="15463" xr2:uid="{03DD5425-0ECE-42AD-87FB-24C50220D827}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Float32Array</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>(reinterpret above)</t>
+  </si>
+  <si>
+    <t>_mm256_packs_epi32?</t>
+  </si>
+  <si>
+    <t>_mm256_packs_epi8?</t>
   </si>
 </sst>
 </file>
@@ -184,12 +190,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,32 +350,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -374,24 +371,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -422,10 +401,46 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -768,45 +783,45 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.3828125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.69140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.4609375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.15234375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.4609375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.3828125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.15234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.4609375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.15234375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.765625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -817,163 +832,178 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B3" s="14"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="15" t="s">
         <v>27</v>
       </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B4" s="14"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="15"/>
-      <c r="C5" s="11">
+    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="25"/>
+      <c r="C5" s="19">
         <v>4</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="25"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="15" t="s">
         <v>28</v>
       </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="25"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="29">
+    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="28">
         <v>4</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="8" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="4" t="s">
+      <c r="D11" s="27"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B12" s="16"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="17">
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="31">
         <v>8</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="7">
         <v>4</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11">
+      <c r="D13" s="29"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19">
         <v>8</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
     </row>
@@ -981,100 +1011,100 @@
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="D14" s="8" t="s">
+      <c r="B14" s="8"/>
+      <c r="D14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="27"/>
+      <c r="F14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B16" s="18"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="19"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="B16" s="8"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="9"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="D18" s="25"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="8" t="s">
+      <c r="B18" s="10"/>
+      <c r="D18" s="15"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B19" s="20"/>
-      <c r="D19" s="25" t="s">
+      <c r="B19" s="10"/>
+      <c r="D19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="4" t="s">
+      <c r="F19" s="27"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="20"/>
-      <c r="D20" s="25"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="21"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="26">
-        <v>8</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11">
+      <c r="B20" s="10"/>
+      <c r="D20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+    </row>
+    <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="11"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19">
         <v>16</v>
       </c>
     </row>
@@ -1082,120 +1112,122 @@
       <c r="A22" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="F22" s="8" t="s">
+      <c r="B22" s="10"/>
+      <c r="F22" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="4" t="s">
+      <c r="G22" s="27"/>
+      <c r="H22" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="18" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="20"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="B23" s="10"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B24" s="20"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="21"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="B24" s="10"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+    </row>
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="11"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="D26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="8" t="s">
+      <c r="B26" s="10"/>
+      <c r="D26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B27" s="20"/>
-      <c r="D27" s="25" t="s">
+      <c r="B27" s="10"/>
+      <c r="D27" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="8"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B28" s="20"/>
-      <c r="D28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="8"/>
-    </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="21"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="12"/>
+      <c r="B28" s="10"/>
+      <c r="D28" s="15"/>
+      <c r="F28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="27"/>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="11"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="H30" s="8" t="s">
+      <c r="B30" s="10"/>
+      <c r="H30" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="I30" s="5"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B31" s="20"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="5"/>
+      <c r="B31" s="10"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B32" s="20"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="5"/>
+      <c r="B32" s="10"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B33" s="21"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="35" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="14" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>